<commit_message>
1. 增加了使用IoT数据集，用来做domain generalization和adaption； 2. 增加了使用DeepSAD和ensemble方法来进行domain generalization的代码。
</commit_message>
<xml_diff>
--- a/auxiliary_data_AD/log/example/性能比较.xlsx
+++ b/auxiliary_data_AD/log/example/性能比较.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\Yukina\Missile_Fault_Detection\project\auxiliary_data_AD\log\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97A3EE8F-A3A6-4322-A922-AAA9AC22C719}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7294976B-B3E5-4080-AC3C-1F1619E7815A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="aucroc" sheetId="1" r:id="rId1"/>
     <sheet name="aucroc_all" sheetId="3" r:id="rId2"/>
     <sheet name="aucpr" sheetId="2" r:id="rId3"/>
+    <sheet name="PANDA" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="71">
   <si>
     <t>origin</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -288,6 +289,23 @@
     <t>layer</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>cutmix-0.7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cutmix-0.8</t>
+  </si>
+  <si>
+    <t>cutmix-0.9</t>
+  </si>
+  <si>
+    <t>PANDA_origin_resnet50</t>
+  </si>
+  <si>
+    <t>PANDA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -435,7 +453,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -521,6 +539,9 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1741,6 +1762,77 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1596591" cy="609013"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="16" name="文本框 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9BFC38AD-C0B1-4FCE-A281-125E28671A3F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="23402925" y="3429000"/>
+          <a:ext cx="1596591" cy="609013"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+            <a:t>backbone=resnet50,</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+            <a:t>MLP_dim=(512,256,128)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+            <a:t>layer=3</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2966,8 +3058,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EF0B9D7-C782-4349-877D-53CE90DBDC85}">
   <dimension ref="A1:AS110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AF26" sqref="AF26"/>
+    <sheetView topLeftCell="W1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Y17" sqref="Y17:Y19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2976,7 +3068,7 @@
     <col min="26" max="26" width="9.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A1" s="4"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -3051,8 +3143,23 @@
       <c r="AE1" s="4" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="AH1" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="AI1" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="AJ1" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="AK1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="AL1" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -3132,8 +3239,26 @@
       <c r="AE2">
         <v>0.93380952399999995</v>
       </c>
-    </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="AH2">
+        <v>0.99960317499999995</v>
+      </c>
+      <c r="AI2">
+        <v>0.99920634900000005</v>
+      </c>
+      <c r="AJ2">
+        <v>0.99722222199999999</v>
+      </c>
+      <c r="AK2">
+        <v>0.99007936500000004</v>
+      </c>
+      <c r="AL2">
+        <v>0.990873016</v>
+      </c>
+      <c r="AO2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -3213,8 +3338,23 @@
       <c r="AE3">
         <v>0.80982008999999999</v>
       </c>
-    </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="AH3">
+        <v>0.81634182899999996</v>
+      </c>
+      <c r="AI3">
+        <v>0.82683658199999999</v>
+      </c>
+      <c r="AJ3">
+        <v>0.82130809599999999</v>
+      </c>
+      <c r="AK3">
+        <v>0.80416041999999999</v>
+      </c>
+      <c r="AL3">
+        <v>0.78635682200000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -3294,8 +3434,23 @@
       <c r="AE4">
         <v>0.80973274799999995</v>
       </c>
-    </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="AH4">
+        <v>0.82568807300000002</v>
+      </c>
+      <c r="AI4">
+        <v>0.80714000799999996</v>
+      </c>
+      <c r="AJ4">
+        <v>0.80773833299999998</v>
+      </c>
+      <c r="AK4">
+        <v>0.80674112499999995</v>
+      </c>
+      <c r="AL4">
+        <v>0.77622656599999995</v>
+      </c>
+    </row>
+    <row r="5" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -3375,8 +3530,23 @@
       <c r="AE5">
         <v>0.97656500800000001</v>
       </c>
-    </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="AH5">
+        <v>0.75240770499999998</v>
+      </c>
+      <c r="AI5">
+        <v>0.75341091500000001</v>
+      </c>
+      <c r="AJ5">
+        <v>0.80096308199999999</v>
+      </c>
+      <c r="AK5">
+        <v>0.68459068999999995</v>
+      </c>
+      <c r="AL5">
+        <v>0.64666934200000004</v>
+      </c>
+    </row>
+    <row r="6" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>27</v>
       </c>
@@ -3456,8 +3626,23 @@
       <c r="AE6">
         <v>0.52631578899999998</v>
       </c>
-    </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="AH6">
+        <v>0.479114453</v>
+      </c>
+      <c r="AI6">
+        <v>0.433166249</v>
+      </c>
+      <c r="AJ6">
+        <v>0.43441938200000002</v>
+      </c>
+      <c r="AK6">
+        <v>0.45446950699999999</v>
+      </c>
+      <c r="AL6">
+        <v>0.44110275700000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
@@ -3537,8 +3722,23 @@
       <c r="AE7">
         <v>0.86628571399999998</v>
       </c>
-    </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="AH7">
+        <v>0.84142857100000001</v>
+      </c>
+      <c r="AI7">
+        <v>0.86928571399999999</v>
+      </c>
+      <c r="AJ7">
+        <v>0.91749999999999998</v>
+      </c>
+      <c r="AK7">
+        <v>0.88446428600000004</v>
+      </c>
+      <c r="AL7">
+        <v>0.83089285700000004</v>
+      </c>
+    </row>
+    <row r="8" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
@@ -3618,8 +3818,23 @@
       <c r="AE8">
         <v>0.99171195700000003</v>
       </c>
-    </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="AH8">
+        <v>0.99048913000000005</v>
+      </c>
+      <c r="AI8">
+        <v>0.99490489100000001</v>
+      </c>
+      <c r="AJ8">
+        <v>0.99150815199999998</v>
+      </c>
+      <c r="AK8">
+        <v>0.99388586999999995</v>
+      </c>
+      <c r="AL8">
+        <v>0.99643342400000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
@@ -3699,8 +3914,23 @@
       <c r="AE9">
         <v>0.61964809399999998</v>
       </c>
-    </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="AH9">
+        <v>0.87438905200000006</v>
+      </c>
+      <c r="AI9">
+        <v>0.882209189</v>
+      </c>
+      <c r="AJ9">
+        <v>0.87218963800000004</v>
+      </c>
+      <c r="AK9">
+        <v>0.89125122199999995</v>
+      </c>
+      <c r="AL9">
+        <v>0.89149560100000003</v>
+      </c>
+    </row>
+    <row r="10" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
@@ -3780,8 +4010,23 @@
       <c r="AE10">
         <v>0.71369339899999995</v>
       </c>
-    </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="AH10">
+        <v>0.70649208900000005</v>
+      </c>
+      <c r="AI10">
+        <v>0.71849427200000004</v>
+      </c>
+      <c r="AJ10">
+        <v>0.72490452800000005</v>
+      </c>
+      <c r="AK10">
+        <v>0.62370431000000004</v>
+      </c>
+      <c r="AL10">
+        <v>0.65684669900000003</v>
+      </c>
+    </row>
+    <row r="11" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>28</v>
       </c>
@@ -3861,8 +4106,23 @@
       <c r="AE11">
         <v>0.63980323800000005</v>
       </c>
-    </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="AH11">
+        <v>0.53084648499999998</v>
+      </c>
+      <c r="AI11">
+        <v>0.538327526</v>
+      </c>
+      <c r="AJ11">
+        <v>0.49877023999999998</v>
+      </c>
+      <c r="AK11">
+        <v>0.53986472600000002</v>
+      </c>
+      <c r="AL11">
+        <v>0.47550727599999998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
@@ -3942,8 +4202,23 @@
       <c r="AE12">
         <v>0.97344877299999999</v>
       </c>
-    </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="AH12">
+        <v>0.96284271300000002</v>
+      </c>
+      <c r="AI12">
+        <v>0.969877345</v>
+      </c>
+      <c r="AJ12">
+        <v>0.962121212</v>
+      </c>
+      <c r="AK12">
+        <v>0.96464646499999995</v>
+      </c>
+      <c r="AL12">
+        <v>0.97041847000000003</v>
+      </c>
+    </row>
+    <row r="13" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
@@ -4023,8 +4298,23 @@
       <c r="AE13">
         <v>0.80722222200000004</v>
       </c>
-    </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="AH13">
+        <v>0.79583333300000003</v>
+      </c>
+      <c r="AI13">
+        <v>0.82638888899999996</v>
+      </c>
+      <c r="AJ13">
+        <v>0.83194444400000001</v>
+      </c>
+      <c r="AK13">
+        <v>0.71805555600000004</v>
+      </c>
+      <c r="AL13">
+        <v>0.68472222199999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
@@ -4104,8 +4394,23 @@
       <c r="AE14">
         <v>0.84916666699999999</v>
       </c>
-    </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="AH14">
+        <v>0.84624999999999995</v>
+      </c>
+      <c r="AI14">
+        <v>0.86604166699999996</v>
+      </c>
+      <c r="AJ14">
+        <v>0.89666666699999997</v>
+      </c>
+      <c r="AK14">
+        <v>0.83875</v>
+      </c>
+      <c r="AL14">
+        <v>0.86583333299999998</v>
+      </c>
+    </row>
+    <row r="15" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>13</v>
       </c>
@@ -4185,8 +4490,23 @@
       <c r="AE15">
         <v>0.97403508800000005</v>
       </c>
-    </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="AH15">
+        <v>0.98289473699999996</v>
+      </c>
+      <c r="AI15">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="AJ15">
+        <v>0.98157894700000003</v>
+      </c>
+      <c r="AK15">
+        <v>0.90701754400000001</v>
+      </c>
+      <c r="AL15">
+        <v>0.82807017500000002</v>
+      </c>
+    </row>
+    <row r="16" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A16" s="11" t="s">
         <v>29</v>
       </c>
@@ -4265,6 +4585,21 @@
       </c>
       <c r="AE16">
         <v>0.93802521000000005</v>
+      </c>
+      <c r="AH16">
+        <v>0.97216386600000004</v>
+      </c>
+      <c r="AI16">
+        <v>0.97610294099999995</v>
+      </c>
+      <c r="AJ16">
+        <v>0.96165966400000003</v>
+      </c>
+      <c r="AK16">
+        <v>0.98476890800000005</v>
+      </c>
+      <c r="AL16">
+        <v>0.98122373900000004</v>
       </c>
     </row>
     <row r="17" spans="1:45" x14ac:dyDescent="0.2">
@@ -4361,7 +4696,7 @@
         <v>0.84568140313333329</v>
       </c>
       <c r="AC17" s="15">
-        <f t="shared" ref="AC17:AE17" si="3">AVERAGE(AC2:AC16)</f>
+        <f t="shared" ref="AC17:AL17" si="3">AVERAGE(AC2:AC16)</f>
         <v>0.81340639353333333</v>
       </c>
       <c r="AD17" s="15">
@@ -4371,6 +4706,28 @@
       <c r="AE17" s="15">
         <f t="shared" si="3"/>
         <v>0.82861890140000005</v>
+      </c>
+      <c r="AF17" s="15"/>
+      <c r="AG17" s="15"/>
+      <c r="AH17" s="15">
+        <f t="shared" si="3"/>
+        <v>0.82511901406666666</v>
+      </c>
+      <c r="AI17" s="15">
+        <f t="shared" si="3"/>
+        <v>0.82909283579999993</v>
+      </c>
+      <c r="AJ17" s="15">
+        <f t="shared" si="3"/>
+        <v>0.83336630713333326</v>
+      </c>
+      <c r="AK17" s="15">
+        <f t="shared" si="3"/>
+        <v>0.80576333293333324</v>
+      </c>
+      <c r="AL17" s="15">
+        <f t="shared" si="3"/>
+        <v>0.78817815326666674</v>
       </c>
     </row>
     <row r="18" spans="1:45" x14ac:dyDescent="0.2">
@@ -4478,6 +4835,28 @@
         <f>AVERAGE(AE5,AE6,AE8,AE12,AE15)</f>
         <v>0.88841532300000003</v>
       </c>
+      <c r="AF18" s="18"/>
+      <c r="AG18" s="18"/>
+      <c r="AH18" s="18">
+        <f t="shared" ref="AF18:AL18" si="5">AVERAGE(AH5,AH6,AH8,AH12,AH15)</f>
+        <v>0.8335497476</v>
+      </c>
+      <c r="AI18" s="18">
+        <f t="shared" si="5"/>
+        <v>0.82527188000000007</v>
+      </c>
+      <c r="AJ18" s="18">
+        <f t="shared" si="5"/>
+        <v>0.83411815499999997</v>
+      </c>
+      <c r="AK18" s="18">
+        <f t="shared" si="5"/>
+        <v>0.80092201519999995</v>
+      </c>
+      <c r="AL18" s="18">
+        <f t="shared" si="5"/>
+        <v>0.77653883359999998</v>
+      </c>
     </row>
     <row r="19" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A19" s="17" t="s">
@@ -4488,31 +4867,31 @@
         <v>0.59424218274865093</v>
       </c>
       <c r="C19" s="18">
-        <f t="shared" ref="C19:I19" si="5">AVERAGE(C2:C4,C7,C9:C11,C13:C14,C16)</f>
+        <f t="shared" ref="C19:I19" si="6">AVERAGE(C2:C4,C7,C9:C11,C13:C14,C16)</f>
         <v>0.60172701377498261</v>
       </c>
       <c r="D19" s="18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.60300963027735899</v>
       </c>
       <c r="E19" s="18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.61604879429999992</v>
       </c>
       <c r="F19" s="18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.63236458458180023</v>
       </c>
       <c r="G19" s="19">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.63666176860852763</v>
       </c>
       <c r="H19" s="18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.62128338230216007</v>
       </c>
       <c r="I19" s="18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.61604879434144499</v>
       </c>
       <c r="J19" s="18">
@@ -4583,6 +4962,28 @@
       <c r="AE19" s="18">
         <f>AVERAGE(AE2:AE4,AE7,AE9:AE11,AE13:AE14,AE16)</f>
         <v>0.79872069059999995</v>
+      </c>
+      <c r="AF19" s="18"/>
+      <c r="AG19" s="18"/>
+      <c r="AH19" s="18">
+        <f t="shared" ref="AF19:AL19" si="7">AVERAGE(AH2:AH4,AH7,AH9:AH11,AH13:AH14,AH16)</f>
+        <v>0.82090364729999998</v>
+      </c>
+      <c r="AI19" s="18">
+        <f t="shared" si="7"/>
+        <v>0.83100331369999991</v>
+      </c>
+      <c r="AJ19" s="18">
+        <f t="shared" si="7"/>
+        <v>0.83299038320000007</v>
+      </c>
+      <c r="AK19" s="18">
+        <f t="shared" si="7"/>
+        <v>0.8081839918</v>
+      </c>
+      <c r="AL19" s="18">
+        <f t="shared" si="7"/>
+        <v>0.79399781310000006</v>
       </c>
     </row>
     <row r="23" spans="1:45" x14ac:dyDescent="0.2">
@@ -4658,11 +5059,11 @@
         <v>0.93790999237223405</v>
       </c>
       <c r="P24" s="2"/>
-      <c r="Q24" s="5"/>
-      <c r="R24" s="12"/>
-      <c r="S24" s="20"/>
-      <c r="T24" s="20"/>
-      <c r="U24" s="20"/>
+      <c r="Q24" s="11"/>
+      <c r="R24" s="11"/>
+      <c r="S24" s="11"/>
+      <c r="T24" s="11"/>
+      <c r="U24" s="11"/>
       <c r="V24" s="21"/>
       <c r="W24" s="21"/>
       <c r="X24" s="2" t="s">
@@ -4752,7 +5153,7 @@
       <c r="K25" s="26">
         <v>0.79697478991596604</v>
       </c>
-      <c r="P25" s="2"/>
+      <c r="P25" s="32"/>
       <c r="Q25" s="1"/>
       <c r="R25" s="2"/>
       <c r="S25" s="20"/>
@@ -4943,7 +5344,7 @@
         <v>0.55165272799681397</v>
       </c>
       <c r="P27" s="2"/>
-      <c r="Q27" s="3"/>
+      <c r="Q27" s="11"/>
       <c r="R27" s="2"/>
       <c r="S27" s="20"/>
       <c r="T27" s="20"/>
@@ -5038,7 +5439,7 @@
         <v>0.74774281805745502</v>
       </c>
       <c r="P28" s="2"/>
-      <c r="Q28" s="3"/>
+      <c r="Q28" s="11"/>
       <c r="R28" s="2"/>
       <c r="S28" s="20"/>
       <c r="T28" s="20"/>
@@ -5133,7 +5534,7 @@
         <v>0.70175824175824097</v>
       </c>
       <c r="P29" s="2"/>
-      <c r="Q29" s="3"/>
+      <c r="Q29" s="11"/>
       <c r="R29" s="2"/>
       <c r="S29" s="20"/>
       <c r="T29" s="20"/>
@@ -5228,7 +5629,7 @@
         <v>0.84483648881239204</v>
       </c>
       <c r="P30" s="2"/>
-      <c r="Q30" s="3"/>
+      <c r="Q30" s="11"/>
       <c r="R30" s="2"/>
       <c r="S30" s="20"/>
       <c r="T30" s="20"/>
@@ -5797,7 +6198,7 @@
       <c r="K36" s="25">
         <v>0.63109756097560898</v>
       </c>
-      <c r="P36" s="2"/>
+      <c r="P36" s="5"/>
       <c r="Q36" s="3"/>
       <c r="R36" s="2"/>
       <c r="S36" s="20"/>
@@ -5892,7 +6293,7 @@
       <c r="K37" s="26">
         <v>0.69972222222222202</v>
       </c>
-      <c r="P37" s="2"/>
+      <c r="P37" s="28"/>
       <c r="Q37" s="1"/>
       <c r="R37" s="2"/>
       <c r="S37" s="20"/>
@@ -5987,7 +6388,7 @@
       <c r="K38" s="25">
         <v>0.62723577235772299</v>
       </c>
-      <c r="P38" s="11"/>
+      <c r="P38" s="20"/>
       <c r="Q38" s="1"/>
       <c r="R38" s="12"/>
       <c r="S38" s="20"/>
@@ -6059,40 +6460,40 @@
         <v>35</v>
       </c>
       <c r="B39" s="16">
-        <f t="shared" ref="B39" si="6">AVERAGE(B24:B38)</f>
+        <f t="shared" ref="B39" si="8">AVERAGE(B24:B38)</f>
         <v>0.66784765492156528</v>
       </c>
       <c r="C39" s="15">
-        <f t="shared" ref="C39" si="7">AVERAGE(C24:C38)</f>
+        <f t="shared" ref="C39" si="9">AVERAGE(C24:C38)</f>
         <v>0.65953465783511322</v>
       </c>
       <c r="D39" s="15">
-        <f t="shared" ref="D39:K39" si="8">AVERAGE(D24:D38)</f>
+        <f t="shared" ref="D39:K39" si="10">AVERAGE(D24:D38)</f>
         <v>0.64689278506666681</v>
       </c>
       <c r="E39" s="15"/>
       <c r="F39" s="15"/>
       <c r="G39" s="15">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0.67988326223415918</v>
       </c>
       <c r="H39" s="15">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0.69184135672437541</v>
       </c>
       <c r="I39" s="16">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0.69868295337342101</v>
       </c>
       <c r="J39" s="16">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0.69641242065446429</v>
       </c>
       <c r="K39" s="16">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0.69411896677682516</v>
       </c>
-      <c r="P39" s="13"/>
+      <c r="P39" s="20"/>
       <c r="Q39" s="15"/>
       <c r="R39" s="15"/>
       <c r="S39" s="15"/>
@@ -6164,40 +6565,40 @@
         <v>32</v>
       </c>
       <c r="B40" s="19">
-        <f t="shared" ref="B40:K40" si="9">AVERAGE(B27,B28,B30,B34,B37)</f>
+        <f t="shared" ref="B40:K40" si="11">AVERAGE(B27,B28,B30,B34,B37)</f>
         <v>0.73021942754764047</v>
       </c>
       <c r="C40" s="18">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.7208786754517984</v>
       </c>
       <c r="D40" s="18">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.70236778420000001</v>
       </c>
       <c r="E40" s="18"/>
       <c r="F40" s="18"/>
       <c r="G40" s="18">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.73676448162575159</v>
       </c>
       <c r="H40" s="18">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.75043945466194328</v>
       </c>
       <c r="I40" s="18">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.74685615018914697</v>
       </c>
       <c r="J40" s="18">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.74363444010851387</v>
       </c>
       <c r="K40" s="18">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.73559085141777669</v>
       </c>
-      <c r="P40" s="17"/>
+      <c r="P40" s="20"/>
       <c r="Q40" s="18"/>
       <c r="R40" s="18"/>
       <c r="S40" s="18"/>
@@ -6217,69 +6618,69 @@
         <v>0.76243860479999992</v>
       </c>
       <c r="AA40" s="15">
-        <f t="shared" ref="AA40:AE40" si="10">AVERAGE(AA25:AA39)</f>
+        <f t="shared" ref="AA40:AE40" si="12">AVERAGE(AA25:AA39)</f>
         <v>0.84314829866666641</v>
       </c>
       <c r="AB40" s="15"/>
       <c r="AC40" s="15">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0.69689745980000006</v>
       </c>
       <c r="AD40" s="15">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0.76989192406666662</v>
       </c>
       <c r="AE40" s="15">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0.86032417953333329</v>
       </c>
       <c r="AF40" s="15">
-        <f t="shared" ref="AF40" si="11">AVERAGE(AF25:AF39)</f>
+        <f t="shared" ref="AF40" si="13">AVERAGE(AF25:AF39)</f>
         <v>0.82670108587649938</v>
       </c>
       <c r="AG40" s="15">
-        <f t="shared" ref="AG40" si="12">AVERAGE(AG25:AG39)</f>
+        <f t="shared" ref="AG40" si="14">AVERAGE(AG25:AG39)</f>
         <v>0.82515507900000007</v>
       </c>
       <c r="AH40" s="15">
-        <f t="shared" ref="AH40" si="13">AVERAGE(AH25:AH39)</f>
+        <f t="shared" ref="AH40" si="15">AVERAGE(AH25:AH39)</f>
         <v>0.79503770946666674</v>
       </c>
       <c r="AI40" s="15">
-        <f t="shared" ref="AI40" si="14">AVERAGE(AI25:AI39)</f>
+        <f t="shared" ref="AI40" si="16">AVERAGE(AI25:AI39)</f>
         <v>0.82655270633333322</v>
       </c>
       <c r="AJ40" s="15">
-        <f t="shared" ref="AJ40" si="15">AVERAGE(AJ25:AJ39)</f>
+        <f t="shared" ref="AJ40" si="17">AVERAGE(AJ25:AJ39)</f>
         <v>0.82521646748490307</v>
       </c>
       <c r="AK40" s="15">
-        <f t="shared" ref="AK40" si="16">AVERAGE(AK25:AK39)</f>
+        <f t="shared" ref="AK40" si="18">AVERAGE(AK25:AK39)</f>
         <v>0.79456156526666666</v>
       </c>
       <c r="AM40" s="15">
-        <f t="shared" ref="AM40" si="17">AVERAGE(AM25:AM39)</f>
+        <f t="shared" ref="AM40" si="19">AVERAGE(AM25:AM39)</f>
         <v>0.72013774679999998</v>
       </c>
       <c r="AN40" s="15">
-        <f t="shared" ref="AN40" si="18">AVERAGE(AN25:AN39)</f>
+        <f t="shared" ref="AN40" si="20">AVERAGE(AN25:AN39)</f>
         <v>0.71504768066666657</v>
       </c>
       <c r="AO40" s="15">
-        <f t="shared" ref="AO40" si="19">AVERAGE(AO25:AO39)</f>
+        <f t="shared" ref="AO40" si="21">AVERAGE(AO25:AO39)</f>
         <v>0.86390112360000004</v>
       </c>
       <c r="AP40" s="15"/>
       <c r="AQ40" s="15">
-        <f t="shared" ref="AQ40" si="20">AVERAGE(AQ25:AQ39)</f>
+        <f t="shared" ref="AQ40" si="22">AVERAGE(AQ25:AQ39)</f>
         <v>0.68880844040000011</v>
       </c>
       <c r="AR40" s="15">
-        <f t="shared" ref="AR40" si="21">AVERAGE(AR25:AR39)</f>
+        <f t="shared" ref="AR40" si="23">AVERAGE(AR25:AR39)</f>
         <v>0.77724544806666673</v>
       </c>
       <c r="AS40" s="15">
-        <f t="shared" ref="AS40" si="22">AVERAGE(AS25:AS39)</f>
+        <f t="shared" ref="AS40" si="24">AVERAGE(AS25:AS39)</f>
         <v>0.85844981413333343</v>
       </c>
     </row>
@@ -6288,37 +6689,37 @@
         <v>33</v>
       </c>
       <c r="B41" s="19">
-        <f t="shared" ref="B41:K41" si="23">AVERAGE(B24:B26,B29,B31:B33,B35:B36,B38)</f>
+        <f t="shared" ref="B41:K41" si="25">AVERAGE(B24:B26,B29,B31:B33,B35:B36,B38)</f>
         <v>0.63666176860852763</v>
       </c>
       <c r="C41" s="18">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>0.6288626490267708</v>
       </c>
       <c r="D41" s="18">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>0.61915528549999999</v>
       </c>
       <c r="E41" s="18"/>
       <c r="F41" s="18"/>
       <c r="G41" s="18">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>0.65144265253836298</v>
       </c>
       <c r="H41" s="18">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>0.66254230775559153</v>
       </c>
       <c r="I41" s="18">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>0.67459635496555814</v>
       </c>
       <c r="J41" s="18">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>0.67280141092743961</v>
       </c>
       <c r="K41" s="18">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>0.67338302445634923</v>
       </c>
       <c r="P41" s="17"/>
@@ -6341,68 +6742,68 @@
         <v>0.6646561151999999</v>
       </c>
       <c r="AA41" s="18">
-        <f t="shared" ref="AA41:AK41" si="24">AVERAGE(AA28,AA29,AA31,AA35,AA38)</f>
+        <f t="shared" ref="AA41:AK41" si="26">AVERAGE(AA28,AA29,AA31,AA35,AA38)</f>
         <v>0.80362691280000009</v>
       </c>
       <c r="AB41" s="18"/>
       <c r="AC41" s="18">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>0.61204013059999995</v>
       </c>
       <c r="AD41" s="18">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>0.68887916400000004</v>
       </c>
       <c r="AE41" s="18">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>0.8761972414000001</v>
       </c>
       <c r="AF41" s="18">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>0.85549034736782337</v>
       </c>
       <c r="AG41" s="18">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>0.83789154880000005</v>
       </c>
       <c r="AH41" s="18">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>0.80484691019999999</v>
       </c>
       <c r="AI41" s="18">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>0.85522094360000001</v>
       </c>
       <c r="AJ41" s="18">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>0.83757845929153851</v>
       </c>
       <c r="AK41" s="18">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>0.80485736379999984</v>
       </c>
       <c r="AM41" s="18">
-        <f t="shared" ref="AM41:AO41" si="25">AVERAGE(AM28,AM29,AM31,AM35,AM38)</f>
+        <f t="shared" ref="AM41:AO41" si="27">AVERAGE(AM28,AM29,AM31,AM35,AM38)</f>
         <v>0.6710244432000001</v>
       </c>
       <c r="AN41" s="18">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>0.61180592980000004</v>
       </c>
       <c r="AO41" s="18">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>0.88104034819999999</v>
       </c>
       <c r="AQ41" s="18">
-        <f t="shared" ref="AQ41:AS41" si="26">AVERAGE(AQ28,AQ29,AQ31,AQ35,AQ38)</f>
+        <f t="shared" ref="AQ41:AS41" si="28">AVERAGE(AQ28,AQ29,AQ31,AQ35,AQ38)</f>
         <v>0.60314574659999998</v>
       </c>
       <c r="AR41" s="18">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>0.68862673380000006</v>
       </c>
       <c r="AS41" s="18">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>0.86816653519999998</v>
       </c>
     </row>
@@ -6419,68 +6820,68 @@
         <v>0.8113298496000001</v>
       </c>
       <c r="AA42" s="18">
-        <f t="shared" ref="AA42:AK42" si="27">AVERAGE(AA25:AA27,AA30,AA32:AA34,AA36:AA37,AA39)</f>
+        <f t="shared" ref="AA42:AK42" si="29">AVERAGE(AA25:AA27,AA30,AA32:AA34,AA36:AA37,AA39)</f>
         <v>0.86290899160000001</v>
       </c>
       <c r="AB42" s="18"/>
       <c r="AC42" s="18">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>0.73932612440000001</v>
       </c>
       <c r="AD42" s="18">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>0.81039830409999991</v>
       </c>
       <c r="AE42" s="18">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>0.85238764860000005</v>
       </c>
       <c r="AF42" s="18">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>0.81230645513083766</v>
       </c>
       <c r="AG42" s="18">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>0.81878684409999991</v>
       </c>
       <c r="AH42" s="18">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>0.79013310910000001</v>
       </c>
       <c r="AI42" s="18">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>0.81221858769999999</v>
       </c>
       <c r="AJ42" s="18">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>0.81903547158158541</v>
       </c>
       <c r="AK42" s="18">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>0.78941366599999996</v>
       </c>
       <c r="AM42" s="18">
-        <f t="shared" ref="AM42:AO42" si="28">AVERAGE(AM25:AM27,AM30,AM32:AM34,AM36:AM37,AM39)</f>
+        <f t="shared" ref="AM42:AO42" si="30">AVERAGE(AM25:AM27,AM30,AM32:AM34,AM36:AM37,AM39)</f>
         <v>0.74469439859999986</v>
       </c>
       <c r="AN42" s="18">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>0.76666855610000006</v>
       </c>
       <c r="AO42" s="18">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>0.85533151129999996</v>
       </c>
       <c r="AQ42" s="18">
-        <f t="shared" ref="AQ42:AS42" si="29">AVERAGE(AQ25:AQ27,AQ30,AQ32:AQ34,AQ36:AQ37,AQ39)</f>
+        <f t="shared" ref="AQ42:AS42" si="31">AVERAGE(AQ25:AQ27,AQ30,AQ32:AQ34,AQ36:AQ37,AQ39)</f>
         <v>0.73163978730000001</v>
       </c>
       <c r="AR42" s="18">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>0.8215548051999999</v>
       </c>
       <c r="AS42" s="18">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>0.85359145359999999</v>
       </c>
     </row>
@@ -7895,27 +8296,27 @@
         <v>35</v>
       </c>
       <c r="B61" s="15">
-        <f t="shared" ref="B61:G61" si="30">AVERAGE(B46:B60)</f>
+        <f t="shared" ref="B61:G61" si="32">AVERAGE(B46:B60)</f>
         <v>0.80931271912638947</v>
       </c>
       <c r="C61" s="15">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>0.809652102162145</v>
       </c>
       <c r="D61" s="15">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>0.79941044305917253</v>
       </c>
       <c r="E61" s="15">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>0.79170580456803252</v>
       </c>
       <c r="F61" s="15">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>0.74611674131893002</v>
       </c>
       <c r="G61" s="15">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>0.6091896583782771</v>
       </c>
       <c r="H61" s="15"/>
@@ -7923,27 +8324,27 @@
         <v>35</v>
       </c>
       <c r="K61" s="15">
-        <f t="shared" ref="K61:P61" si="31">AVERAGE(K46:K60)</f>
+        <f t="shared" ref="K61:P61" si="33">AVERAGE(K46:K60)</f>
         <v>0.79379622707226594</v>
       </c>
       <c r="L61" s="15">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>0.79527013670386792</v>
       </c>
       <c r="M61" s="15">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>0.78723862501448394</v>
       </c>
       <c r="N61" s="15">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>0.77883661128904957</v>
       </c>
       <c r="O61" s="15">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>0.73280453251004152</v>
       </c>
       <c r="P61" s="15">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>0.6061540957688708</v>
       </c>
       <c r="R61" s="1"/>
@@ -7998,54 +8399,54 @@
         <v>32</v>
       </c>
       <c r="B62" s="18">
-        <f t="shared" ref="B62:G62" si="32">AVERAGE(B49,B50,B52,B56,B59)</f>
+        <f t="shared" ref="B62:G62" si="34">AVERAGE(B49,B50,B52,B56,B59)</f>
         <v>0.86045660702837989</v>
       </c>
       <c r="C62" s="18">
-        <f t="shared" si="32"/>
+        <f t="shared" si="34"/>
         <v>0.85745606961350374</v>
       </c>
       <c r="D62" s="18">
-        <f t="shared" si="32"/>
+        <f t="shared" si="34"/>
         <v>0.84272299971459186</v>
       </c>
       <c r="E62" s="18">
-        <f t="shared" si="32"/>
+        <f t="shared" si="34"/>
         <v>0.83025899099995715</v>
       </c>
       <c r="F62" s="18">
-        <f t="shared" si="32"/>
+        <f t="shared" si="34"/>
         <v>0.76866804528897004</v>
       </c>
       <c r="G62" s="18">
-        <f t="shared" si="32"/>
+        <f t="shared" si="34"/>
         <v>0.59451121577945076</v>
       </c>
       <c r="J62" s="17" t="s">
         <v>32</v>
       </c>
       <c r="K62" s="18">
-        <f t="shared" ref="K62:P62" si="33">AVERAGE(K49,K50,K52,K56,K59)</f>
+        <f t="shared" ref="K62:P62" si="35">AVERAGE(K49,K50,K52,K56,K59)</f>
         <v>0.84688057000485417</v>
       </c>
       <c r="L62" s="18">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>0.85247089654805053</v>
       </c>
       <c r="M62" s="18">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>0.8416008401433821</v>
       </c>
       <c r="N62" s="18">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>0.83659397627494914</v>
       </c>
       <c r="O62" s="18">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>0.78282539867968048</v>
       </c>
       <c r="P62" s="18">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>0.63269527238745338</v>
       </c>
       <c r="R62" s="19"/>
@@ -8057,31 +8458,31 @@
         <v>0.63644329220886242</v>
       </c>
       <c r="U62" s="15">
-        <f t="shared" ref="U62:AA62" si="34">AVERAGE(U47:U61)</f>
+        <f t="shared" ref="U62:AA62" si="36">AVERAGE(U47:U61)</f>
         <v>0.55585844505541815</v>
       </c>
       <c r="V62" s="15">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v>0.55168147506666665</v>
       </c>
       <c r="W62" s="15">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v>0.56096400926666656</v>
       </c>
       <c r="X62" s="15">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v>0.56350728146666662</v>
       </c>
       <c r="Y62" s="15">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v>0.57204028719911881</v>
       </c>
       <c r="Z62" s="15">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v>0.56354796133333329</v>
       </c>
       <c r="AA62" s="15">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v>0.60143095153333326</v>
       </c>
       <c r="AB62" s="15">
@@ -8101,7 +8502,7 @@
         <v>0.64031799680000001</v>
       </c>
       <c r="AF62" s="16">
-        <f t="shared" ref="AF62" si="35">AVERAGE(AF47:AF61)</f>
+        <f t="shared" ref="AF62" si="37">AVERAGE(AF47:AF61)</f>
         <v>0.64661103013333332</v>
       </c>
       <c r="AG62" s="16">
@@ -8114,54 +8515,54 @@
         <v>33</v>
       </c>
       <c r="B63" s="18">
-        <f t="shared" ref="B63:G63" si="36">AVERAGE(B46:B48,B51,B53:B55,B57:B58,B60)</f>
+        <f t="shared" ref="B63:G63" si="38">AVERAGE(B46:B48,B51,B53:B55,B57:B58,B60)</f>
         <v>0.78374077517539431</v>
       </c>
       <c r="C63" s="18">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>0.78575011843646558</v>
       </c>
       <c r="D63" s="18">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>0.77775416473146286</v>
       </c>
       <c r="E63" s="18">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>0.77242921135207021</v>
       </c>
       <c r="F63" s="18">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>0.73484108933391001</v>
       </c>
       <c r="G63" s="18">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>0.61652887967769054</v>
       </c>
       <c r="J63" s="17" t="s">
         <v>33</v>
       </c>
       <c r="K63" s="18">
-        <f t="shared" ref="K63:P63" si="37">AVERAGE(K46:K48,K51,K53:K55,K57:K58,K60)</f>
+        <f t="shared" ref="K63:P63" si="39">AVERAGE(K46:K48,K51,K53:K55,K57:K58,K60)</f>
         <v>0.76725405560597193</v>
       </c>
       <c r="L63" s="18">
-        <f t="shared" si="37"/>
+        <f t="shared" si="39"/>
         <v>0.76666975678177673</v>
       </c>
       <c r="M63" s="18">
-        <f t="shared" si="37"/>
+        <f t="shared" si="39"/>
         <v>0.7600575174500348</v>
       </c>
       <c r="N63" s="18">
-        <f t="shared" si="37"/>
+        <f t="shared" si="39"/>
         <v>0.74995792879609979</v>
       </c>
       <c r="O63" s="18">
-        <f t="shared" si="37"/>
+        <f t="shared" si="39"/>
         <v>0.70779409942522231</v>
       </c>
       <c r="P63" s="18">
-        <f t="shared" si="37"/>
+        <f t="shared" si="39"/>
         <v>0.59288350745957952</v>
       </c>
       <c r="S63" s="17" t="s">
@@ -8172,55 +8573,55 @@
         <v>0.70301900622824642</v>
       </c>
       <c r="U63" s="18">
-        <f t="shared" ref="U63:AA63" si="38">AVERAGE(U50,U51,U53,U57,U60)</f>
+        <f t="shared" ref="U63:AA63" si="40">AVERAGE(U50,U51,U53,U57,U60)</f>
         <v>0.58320991713157999</v>
       </c>
       <c r="V63" s="18">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v>0.55985415379999992</v>
       </c>
       <c r="W63" s="18">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v>0.56804545100000003</v>
       </c>
       <c r="X63" s="18">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v>0.57341046280000008</v>
       </c>
       <c r="Y63" s="18">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v>0.56776325067945455</v>
       </c>
       <c r="Z63" s="18">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v>0.56345668900000001</v>
       </c>
       <c r="AA63" s="18">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v>0.63331710139999997</v>
       </c>
       <c r="AB63" s="18">
-        <f t="shared" ref="AB63:AG63" si="39">AVERAGE(AB50,AB51,AB53,AB57,AB60)</f>
+        <f t="shared" ref="AB63:AG63" si="41">AVERAGE(AB50,AB51,AB53,AB57,AB60)</f>
         <v>0.66044291739999994</v>
       </c>
       <c r="AC63" s="18">
-        <f t="shared" si="39"/>
+        <f t="shared" si="41"/>
         <v>0.70483313140000003</v>
       </c>
       <c r="AD63" s="18">
-        <f t="shared" si="39"/>
+        <f t="shared" si="41"/>
         <v>0.68583976939999991</v>
       </c>
       <c r="AE63" s="18">
-        <f t="shared" si="39"/>
+        <f t="shared" si="41"/>
         <v>0.69969864999999998</v>
       </c>
       <c r="AF63" s="18">
-        <f t="shared" si="39"/>
+        <f t="shared" si="41"/>
         <v>0.7041091478</v>
       </c>
       <c r="AG63" s="18">
-        <f t="shared" si="39"/>
+        <f t="shared" si="41"/>
         <v>0.7067299078</v>
       </c>
     </row>
@@ -8233,55 +8634,55 @@
         <v>0.60315543519917048</v>
       </c>
       <c r="U64" s="18">
-        <f t="shared" ref="U64:AA64" si="40">AVERAGE(U47:U49,U52,U54:U56,U58:U59,U61)</f>
+        <f t="shared" ref="U64:AA64" si="42">AVERAGE(U47:U49,U52,U54:U56,U58:U59,U61)</f>
         <v>0.54218270901733701</v>
       </c>
       <c r="V64" s="18">
-        <f t="shared" si="40"/>
+        <f t="shared" si="42"/>
         <v>0.54759513569999996</v>
       </c>
       <c r="W64" s="18">
-        <f t="shared" si="40"/>
+        <f t="shared" si="42"/>
         <v>0.55742328839999999</v>
       </c>
       <c r="X64" s="18">
-        <f t="shared" si="40"/>
+        <f t="shared" si="42"/>
         <v>0.5585556908</v>
       </c>
       <c r="Y64" s="18">
-        <f t="shared" si="40"/>
+        <f t="shared" si="42"/>
         <v>0.57417880545895095</v>
       </c>
       <c r="Z64" s="18">
-        <f t="shared" si="40"/>
+        <f t="shared" si="42"/>
         <v>0.56359359749999993</v>
       </c>
       <c r="AA64" s="18">
-        <f t="shared" si="40"/>
+        <f t="shared" si="42"/>
         <v>0.58548787660000001</v>
       </c>
       <c r="AB64" s="18">
-        <f t="shared" ref="AB64:AG64" si="41">AVERAGE(AB47:AB49,AB52,AB54:AB56,AB58:AB59,AB61)</f>
+        <f t="shared" ref="AB64:AG64" si="43">AVERAGE(AB47:AB49,AB52,AB54:AB56,AB58:AB59,AB61)</f>
         <v>0.6110833631999999</v>
       </c>
       <c r="AC64" s="18">
-        <f t="shared" si="41"/>
+        <f t="shared" si="43"/>
         <v>0.62084230320000011</v>
       </c>
       <c r="AD64" s="18">
-        <f t="shared" si="41"/>
+        <f t="shared" si="43"/>
         <v>0.59808727559999997</v>
       </c>
       <c r="AE64" s="18">
-        <f t="shared" si="41"/>
+        <f t="shared" si="43"/>
         <v>0.61062767020000008</v>
       </c>
       <c r="AF64" s="18">
-        <f t="shared" si="41"/>
+        <f t="shared" si="43"/>
         <v>0.61786197129999998</v>
       </c>
       <c r="AG64" s="18">
-        <f t="shared" si="41"/>
+        <f t="shared" si="43"/>
         <v>0.61459326130000014</v>
       </c>
     </row>
@@ -8460,55 +8861,55 @@
         <v>0.6573960097999999</v>
       </c>
       <c r="U85" s="15" t="e">
-        <f t="shared" ref="U85:AG85" si="42">AVERAGE(U70:U84)</f>
+        <f t="shared" ref="U85:AG85" si="44">AVERAGE(U70:U84)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="V85" s="15" t="e">
-        <f t="shared" si="42"/>
+        <f t="shared" si="44"/>
         <v>#DIV/0!</v>
       </c>
       <c r="W85" s="15" t="e">
-        <f t="shared" si="42"/>
+        <f t="shared" si="44"/>
         <v>#DIV/0!</v>
       </c>
       <c r="X85" s="15" t="e">
-        <f t="shared" si="42"/>
+        <f t="shared" si="44"/>
         <v>#DIV/0!</v>
       </c>
       <c r="Y85" s="15" t="e">
-        <f t="shared" si="42"/>
+        <f t="shared" si="44"/>
         <v>#DIV/0!</v>
       </c>
       <c r="Z85" s="15" t="e">
-        <f t="shared" si="42"/>
+        <f t="shared" si="44"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AA85" s="15" t="e">
-        <f t="shared" si="42"/>
+        <f t="shared" si="44"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB85" s="15" t="e">
-        <f t="shared" si="42"/>
+        <f t="shared" si="44"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AC85" s="15" t="e">
-        <f t="shared" si="42"/>
+        <f t="shared" si="44"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AD85" s="15" t="e">
-        <f t="shared" si="42"/>
+        <f t="shared" si="44"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AE85" s="15" t="e">
-        <f t="shared" si="42"/>
+        <f t="shared" si="44"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AF85" s="15" t="e">
-        <f t="shared" si="42"/>
+        <f t="shared" si="44"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AG85" s="15" t="e">
-        <f t="shared" si="42"/>
+        <f t="shared" si="44"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -8522,55 +8923,55 @@
         <v>0.71097019680000006</v>
       </c>
       <c r="U86" s="18" t="e">
-        <f t="shared" ref="U86:AG86" si="43">AVERAGE(U73,U74,U76,U80,U83)</f>
+        <f t="shared" ref="U86:AG86" si="45">AVERAGE(U73,U74,U76,U80,U83)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="V86" s="18" t="e">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v>#DIV/0!</v>
       </c>
       <c r="W86" s="18" t="e">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v>#DIV/0!</v>
       </c>
       <c r="X86" s="18" t="e">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v>#DIV/0!</v>
       </c>
       <c r="Y86" s="18" t="e">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v>#DIV/0!</v>
       </c>
       <c r="Z86" s="18" t="e">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AA86" s="18" t="e">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB86" s="18" t="e">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AC86" s="18" t="e">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AD86" s="18" t="e">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AE86" s="18" t="e">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AF86" s="18" t="e">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AG86" s="18" t="e">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -8584,55 +8985,55 @@
         <v>0.63060891629999993</v>
       </c>
       <c r="U87" s="18" t="e">
-        <f t="shared" ref="U87:AG87" si="44">AVERAGE(U70:U72,U75,U77:U79,U81:U82,U84)</f>
+        <f t="shared" ref="U87:AG87" si="46">AVERAGE(U70:U72,U75,U77:U79,U81:U82,U84)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="V87" s="18" t="e">
-        <f t="shared" si="44"/>
+        <f t="shared" si="46"/>
         <v>#DIV/0!</v>
       </c>
       <c r="W87" s="18" t="e">
-        <f t="shared" si="44"/>
+        <f t="shared" si="46"/>
         <v>#DIV/0!</v>
       </c>
       <c r="X87" s="18" t="e">
-        <f t="shared" si="44"/>
+        <f t="shared" si="46"/>
         <v>#DIV/0!</v>
       </c>
       <c r="Y87" s="18" t="e">
-        <f t="shared" si="44"/>
+        <f t="shared" si="46"/>
         <v>#DIV/0!</v>
       </c>
       <c r="Z87" s="18" t="e">
-        <f t="shared" si="44"/>
+        <f t="shared" si="46"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AA87" s="18" t="e">
-        <f t="shared" si="44"/>
+        <f t="shared" si="46"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AB87" s="18" t="e">
-        <f t="shared" si="44"/>
+        <f t="shared" si="46"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AC87" s="18" t="e">
-        <f t="shared" si="44"/>
+        <f t="shared" si="46"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AD87" s="18" t="e">
-        <f t="shared" si="44"/>
+        <f t="shared" si="46"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AE87" s="18" t="e">
-        <f t="shared" si="44"/>
+        <f t="shared" si="46"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AF87" s="18" t="e">
-        <f t="shared" si="44"/>
+        <f t="shared" si="46"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AG87" s="18" t="e">
-        <f t="shared" si="44"/>
+        <f t="shared" si="46"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -9490,63 +9891,63 @@
         <v>0.67064627446666658</v>
       </c>
       <c r="S108" s="15">
-        <f t="shared" ref="S108" si="45">AVERAGE(S93:S107)</f>
+        <f t="shared" ref="S108" si="47">AVERAGE(S93:S107)</f>
         <v>0.62949090613333347</v>
       </c>
       <c r="T108" s="15">
-        <f t="shared" ref="T108" si="46">AVERAGE(T93:T107)</f>
+        <f t="shared" ref="T108" si="48">AVERAGE(T93:T107)</f>
         <v>0.64394546133333319</v>
       </c>
       <c r="U108" s="15">
-        <f t="shared" ref="U108" si="47">AVERAGE(U93:U107)</f>
+        <f t="shared" ref="U108" si="49">AVERAGE(U93:U107)</f>
         <v>0.65824788373333332</v>
       </c>
       <c r="V108" s="15">
-        <f t="shared" ref="V108" si="48">AVERAGE(V93:V107)</f>
+        <f t="shared" ref="V108" si="50">AVERAGE(V93:V107)</f>
         <v>0.67719660699999984</v>
       </c>
       <c r="W108" s="15">
-        <f t="shared" ref="W108" si="49">AVERAGE(W93:W107)</f>
+        <f t="shared" ref="W108" si="51">AVERAGE(W93:W107)</f>
         <v>0.68466025874297654</v>
       </c>
       <c r="X108" s="15">
-        <f t="shared" ref="X108" si="50">AVERAGE(X93:X107)</f>
+        <f t="shared" ref="X108" si="52">AVERAGE(X93:X107)</f>
         <v>0.69057057233333341</v>
       </c>
       <c r="Y108" s="15">
-        <f t="shared" ref="Y108" si="51">AVERAGE(Y93:Y107)</f>
+        <f t="shared" ref="Y108" si="53">AVERAGE(Y93:Y107)</f>
         <v>0.67447751519999999</v>
       </c>
       <c r="Z108" s="15">
-        <f t="shared" ref="Z108" si="52">AVERAGE(Z93:Z107)</f>
+        <f t="shared" ref="Z108" si="54">AVERAGE(Z93:Z107)</f>
         <v>0.64394546133333319</v>
       </c>
       <c r="AA108" s="15">
-        <f t="shared" ref="AA108" si="53">AVERAGE(AA93:AA107)</f>
+        <f t="shared" ref="AA108" si="55">AVERAGE(AA93:AA107)</f>
         <v>0.65707601426666673</v>
       </c>
       <c r="AB108" s="15">
-        <f t="shared" ref="AB108" si="54">AVERAGE(AB93:AB107)</f>
+        <f t="shared" ref="AB108" si="56">AVERAGE(AB93:AB107)</f>
         <v>0.67373057366666667</v>
       </c>
       <c r="AC108" s="15">
-        <f t="shared" ref="AC108" si="55">AVERAGE(AC93:AC107)</f>
+        <f t="shared" ref="AC108" si="57">AVERAGE(AC93:AC107)</f>
         <v>0.68847724459999993</v>
       </c>
       <c r="AD108" s="16">
-        <f t="shared" ref="AD108" si="56">AVERAGE(AD93:AD107)</f>
+        <f t="shared" ref="AD108" si="58">AVERAGE(AD93:AD107)</f>
         <v>0.71734000119999997</v>
       </c>
       <c r="AE108" s="15">
-        <f t="shared" ref="AE108" si="57">AVERAGE(AE93:AE107)</f>
+        <f t="shared" ref="AE108" si="59">AVERAGE(AE93:AE107)</f>
         <v>0.7166698888666666</v>
       </c>
       <c r="AF108" s="15">
-        <f t="shared" ref="AF108" si="58">AVERAGE(AF93:AF107)</f>
+        <f t="shared" ref="AF108" si="60">AVERAGE(AF93:AF107)</f>
         <v>0.71615877393333349</v>
       </c>
       <c r="AG108" s="15">
-        <f t="shared" ref="AG108" si="59">AVERAGE(AG93:AG107)</f>
+        <f t="shared" ref="AG108" si="61">AVERAGE(AG93:AG107)</f>
         <v>0.70804667119999998</v>
       </c>
     </row>
@@ -9559,63 +9960,63 @@
         <v>0.72139350120000001</v>
       </c>
       <c r="S109" s="18">
-        <f t="shared" ref="S109:Y109" si="60">AVERAGE(S96,S97,S99,S103,S106)</f>
+        <f t="shared" ref="S109:Y109" si="62">AVERAGE(S96,S97,S99,S103,S106)</f>
         <v>0.58692838540000003</v>
       </c>
       <c r="T109" s="18">
-        <f t="shared" si="60"/>
+        <f t="shared" si="62"/>
         <v>0.63279722820000006</v>
       </c>
       <c r="U109" s="18">
-        <f t="shared" si="60"/>
+        <f t="shared" si="62"/>
         <v>0.67168361160000001</v>
       </c>
       <c r="V109" s="18">
-        <f t="shared" si="60"/>
+        <f t="shared" si="62"/>
         <v>0.71707277780000001</v>
       </c>
       <c r="W109" s="18">
-        <f t="shared" si="60"/>
+        <f t="shared" si="62"/>
         <v>0.71218243347964927</v>
       </c>
       <c r="X109" s="18">
-        <f t="shared" si="60"/>
+        <f t="shared" si="62"/>
         <v>0.73489502179999999</v>
       </c>
       <c r="Y109" s="18">
-        <f t="shared" si="60"/>
+        <f t="shared" si="62"/>
         <v>0.75902896760000005</v>
       </c>
       <c r="Z109" s="18">
-        <f t="shared" ref="Z109:AG109" si="61">AVERAGE(Z96,Z97,Z99,Z103,Z106)</f>
+        <f t="shared" ref="Z109:AG109" si="63">AVERAGE(Z96,Z97,Z99,Z103,Z106)</f>
         <v>0.63279722820000006</v>
       </c>
       <c r="AA109" s="18">
-        <f t="shared" si="61"/>
+        <f t="shared" si="63"/>
         <v>0.667088809</v>
       </c>
       <c r="AB109" s="18">
-        <f t="shared" si="61"/>
+        <f t="shared" si="63"/>
         <v>0.69975922140000002</v>
       </c>
       <c r="AC109" s="18">
-        <f t="shared" si="61"/>
+        <f t="shared" si="63"/>
         <v>0.72835684359999997</v>
       </c>
       <c r="AD109" s="18">
-        <f t="shared" si="61"/>
+        <f t="shared" si="63"/>
         <v>0.76954440319999995</v>
       </c>
       <c r="AE109" s="18">
-        <f t="shared" si="61"/>
+        <f t="shared" si="63"/>
         <v>0.79338690580000004</v>
       </c>
       <c r="AF109" s="18">
-        <f t="shared" si="61"/>
+        <f t="shared" si="63"/>
         <v>0.81129303660000007</v>
       </c>
       <c r="AG109" s="18">
-        <f t="shared" si="61"/>
+        <f t="shared" si="63"/>
         <v>0.79579568080000007</v>
       </c>
     </row>
@@ -9628,63 +10029,63 @@
         <v>0.64527266110000014</v>
       </c>
       <c r="S110" s="18">
-        <f t="shared" ref="S110:Y110" si="62">AVERAGE(S93:S95,S98,S100:S102,S104:S105,S107)</f>
+        <f t="shared" ref="S110:Y110" si="64">AVERAGE(S93:S95,S98,S100:S102,S104:S105,S107)</f>
         <v>0.65077216650000003</v>
       </c>
       <c r="T110" s="18">
-        <f t="shared" si="62"/>
+        <f t="shared" si="64"/>
         <v>0.64951957790000003</v>
       </c>
       <c r="U110" s="18">
-        <f t="shared" si="62"/>
+        <f t="shared" si="64"/>
         <v>0.65153001980000003</v>
       </c>
       <c r="V110" s="18">
-        <f t="shared" si="62"/>
+        <f t="shared" si="64"/>
         <v>0.65725852159999998</v>
       </c>
       <c r="W110" s="18">
-        <f t="shared" si="62"/>
+        <f t="shared" si="64"/>
         <v>0.67089917137463995</v>
       </c>
       <c r="X110" s="18">
-        <f t="shared" si="62"/>
+        <f t="shared" si="64"/>
         <v>0.66840834760000001</v>
       </c>
       <c r="Y110" s="18">
-        <f t="shared" si="62"/>
+        <f t="shared" si="64"/>
         <v>0.63220178900000001</v>
       </c>
       <c r="Z110" s="18">
-        <f t="shared" ref="Z110:AG110" si="63">AVERAGE(Z93:Z95,Z98,Z100:Z102,Z104:Z105,Z107)</f>
+        <f t="shared" ref="Z110:AG110" si="65">AVERAGE(Z93:Z95,Z98,Z100:Z102,Z104:Z105,Z107)</f>
         <v>0.64951957790000003</v>
       </c>
       <c r="AA110" s="18">
-        <f t="shared" si="63"/>
+        <f t="shared" si="65"/>
         <v>0.65206961690000009</v>
       </c>
       <c r="AB110" s="18">
-        <f t="shared" si="63"/>
+        <f t="shared" si="65"/>
         <v>0.66071624979999988</v>
       </c>
       <c r="AC110" s="18">
-        <f t="shared" si="63"/>
+        <f t="shared" si="65"/>
         <v>0.66853744510000013</v>
       </c>
       <c r="AD110" s="18">
-        <f t="shared" si="63"/>
+        <f t="shared" si="65"/>
         <v>0.69123780020000003</v>
       </c>
       <c r="AE110" s="18">
-        <f t="shared" si="63"/>
+        <f t="shared" si="65"/>
         <v>0.67831138040000005</v>
       </c>
       <c r="AF110" s="18">
-        <f t="shared" si="63"/>
+        <f t="shared" si="65"/>
         <v>0.66859164260000004</v>
       </c>
       <c r="AG110" s="18">
-        <f t="shared" si="63"/>
+        <f t="shared" si="65"/>
         <v>0.66417216639999999</v>
       </c>
     </row>
@@ -9701,7 +10102,7 @@
   <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -10234,4 +10635,292 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{086EED24-41B4-4275-839F-DF40BA3574B8}">
+  <dimension ref="A1:D19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L20" sqref="L20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B1" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="4">
+        <v>0.98769841300000005</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0.98888888888888804</v>
+      </c>
+      <c r="D2">
+        <v>0.97777777799999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="4">
+        <v>0.79010494799999997</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0.814374062968515</v>
+      </c>
+      <c r="D3">
+        <v>0.84182908499999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="4">
+        <v>0.73992820100000001</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0.739928201037096</v>
+      </c>
+      <c r="D4">
+        <v>0.79158356600000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="4">
+        <v>0.88543338699999996</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0.94642857142857095</v>
+      </c>
+      <c r="D5">
+        <v>0.87219101099999996</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="4">
+        <v>0.34043441899999999</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0.72263993316624897</v>
+      </c>
+      <c r="D6">
+        <v>0.39306599800000003</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4">
+        <v>0.90785714299999998</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0.92232142857142796</v>
+      </c>
+      <c r="D7">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="4">
+        <v>0.994565217</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0.99864130434782505</v>
+      </c>
+      <c r="D8">
+        <v>0.99796195700000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="4">
+        <v>0.70234604099999998</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0.70087976539589403</v>
+      </c>
+      <c r="D9">
+        <v>0.84139784900000003</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="4">
+        <v>0.765821058</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0.74031642116748497</v>
+      </c>
+      <c r="D10">
+        <v>0.75913802500000005</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="4">
+        <v>0.49579831899999999</v>
+      </c>
+      <c r="C11" s="1">
+        <v>0.48585775773724099</v>
+      </c>
+      <c r="D11">
+        <v>0.40069686399999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="4">
+        <v>0.96897546899999998</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0.98178210678210598</v>
+      </c>
+      <c r="D12">
+        <v>0.97528859999999995</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="4">
+        <v>0.89722222200000001</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0.87083333333333302</v>
+      </c>
+      <c r="D13">
+        <v>0.876388889</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="4">
+        <v>0.74124999999999996</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0.83041666666666603</v>
+      </c>
+      <c r="D14">
+        <v>0.72916666699999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="4">
+        <v>0.96491228100000004</v>
+      </c>
+      <c r="C15" s="1">
+        <v>0.99429824561403501</v>
+      </c>
+      <c r="D15">
+        <v>0.92456140399999998</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="4">
+        <v>0.96179096600000002</v>
+      </c>
+      <c r="C16" s="1">
+        <v>0.97229516806722605</v>
+      </c>
+      <c r="D16">
+        <v>0.98595063000000005</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17" s="15">
+        <f>AVERAGE(B2:B16)</f>
+        <v>0.80960920559999994</v>
+      </c>
+      <c r="C17" s="15">
+        <f t="shared" ref="C17:D17" si="0">AVERAGE(C2:C16)</f>
+        <v>0.84732679034483727</v>
+      </c>
+      <c r="D17" s="15">
+        <f t="shared" si="0"/>
+        <v>0.81779988819999994</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="18">
+        <f>AVERAGE(B5,B6,B8,B12,B15)</f>
+        <v>0.83086415460000007</v>
+      </c>
+      <c r="C18" s="18">
+        <f t="shared" ref="C18:D18" si="1">AVERAGE(C5,C6,C8,C12,C15)</f>
+        <v>0.92875803226775699</v>
+      </c>
+      <c r="D18" s="18">
+        <f t="shared" si="1"/>
+        <v>0.83261379400000002</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" s="18">
+        <f>AVERAGE(B2:B4,B7,B9:B11,B13:B14,B16)</f>
+        <v>0.79898173110000004</v>
+      </c>
+      <c r="C19" s="18">
+        <f t="shared" ref="C19:D19" si="2">AVERAGE(C2:C4,C7,C9:C11,C13:C14,C16)</f>
+        <v>0.80661116938337718</v>
+      </c>
+      <c r="D19" s="18">
+        <f t="shared" si="2"/>
+        <v>0.81039293530000012</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>